<commit_message>
Created gantt chart for sprint 10
</commit_message>
<xml_diff>
--- a/DevelopmentDocuments/Sprints/ganttCharts.xlsx
+++ b/DevelopmentDocuments/Sprints/ganttCharts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agent\Desktop\Projects\PropertyTycoon\DevelopmentDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agent\Desktop\Projects\PropertyTycoon\DevelopmentDocuments\Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C26BE9-9894-4F67-8A3C-AA05E923018B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AFD0A1-5ED9-43A7-98CE-71ACAA4D6355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="9015" windowWidth="38700" windowHeight="15885" firstSheet="3" activeTab="8" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
+    <workbookView xWindow="31545" yWindow="5580" windowWidth="38700" windowHeight="15885" firstSheet="3" activeTab="9" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>Sprint1</t>
   </si>
@@ -260,6 +260,27 @@
   <si>
     <t>Writing documentation</t>
   </si>
+  <si>
+    <t>Complete documentation</t>
+  </si>
+  <si>
+    <t>Finish timed version of game</t>
+  </si>
+  <si>
+    <t>Record video of game being played</t>
+  </si>
+  <si>
+    <t>Make public the GitHub repository</t>
+  </si>
+  <si>
+    <t>Add winning conditions for both versions</t>
+  </si>
+  <si>
+    <t>Make PropertyTycoon logo</t>
+  </si>
+  <si>
+    <t>Create team logo</t>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,6 +354,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -743,6 +767,432 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="88857440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sprint 10</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint10!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint10!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Complete documentation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add winning conditions for both versions</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Finish timed version of game</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Make PropertyTycoon logo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create team logo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Record video of game being played</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Make public the GitHub repository</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint10!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8660-4576-B38D-F236730A9267}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint10!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint10!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Complete documentation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add winning conditions for both versions</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Finish timed version of game</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Make PropertyTycoon logo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create team logo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Record video of game being played</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Make public the GitHub repository</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint10!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8660-4576-B38D-F236730A9267}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="695219136"/>
+        <c:axId val="695218480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="695219136"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="695218480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="695218480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="43966"/>
+          <c:min val="43959"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="695219136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4187,6 +4637,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5051,6 +5541,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -9112,6 +10107,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71CC8AF0-1A23-4D7C-8808-6A77EB5639D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF42399-64A9-49C0-9E7B-BE555B94A2F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9771,11 +10807,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -9895,18 +10931,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537330B-5E37-4C7A-A891-88BB87542914}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -9917,42 +10956,96 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43959</v>
+      </c>
+      <c r="C3" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43960</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43961</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43963</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43963</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43965</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43965</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="5"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C9">
+    <sortCondition ref="B3:B9"/>
+    <sortCondition ref="C3:C9"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9972,11 +11065,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -10080,11 +11173,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -10187,11 +11280,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -10328,11 +11421,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -10445,11 +11538,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -10585,11 +11678,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -10700,11 +11793,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -10805,7 +11898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6F873B-3E4B-4741-9898-256B2E2385F0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
@@ -10815,11 +11908,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">

</xml_diff>